<commit_message>
Korrigiere Projekt- und WBS-ID-Referenzen in der Main.controller.js
</commit_message>
<xml_diff>
--- a/Test_Files/#01_test.xlsx
+++ b/Test_Files/#01_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valdeigm\Downloads\Schedule_testfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valdeigm\OneDrive - Phoron Group GmbH\Projekte\Git\ZETA\z_schedule_app\Test_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B188A6-CB7A-4D2F-96BC-4A81667FC7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6651CAF3-3558-4A85-ABB3-380A0A8D59A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5775" yWindow="8190" windowWidth="29250" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1935" yWindow="9585" windowWidth="29250" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAPUI5 Export" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>projectId</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t>10.20.00019.101</t>
+  </si>
+  <si>
+    <t>10.30.00002</t>
+  </si>
+  <si>
+    <t>10.20.00019</t>
+  </si>
+  <si>
+    <t>10.20.00019.1010103</t>
   </si>
 </sst>
 </file>
@@ -452,11 +461,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -499,7 +508,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -522,7 +531,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -540,6 +549,29 @@
         <v>45780</v>
       </c>
       <c r="H3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2">
+        <v>45719</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45780</v>
+      </c>
+      <c r="E4" s="2">
+        <v>45719</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45780</v>
+      </c>
+      <c r="H4" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>